<commit_message>
Bigmart release note added
</commit_message>
<xml_diff>
--- a/Ordering System/Ekbana.xlsx
+++ b/Ordering System/Ekbana.xlsx
@@ -1505,7 +1505,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
@@ -1977,11 +1977,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AD141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+      <selection activeCell="C142" sqref="C1:C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2206,7 +2205,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="4" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2390,7 +2389,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="6" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2660,7 +2659,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="9" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2734,7 +2733,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2826,7 +2825,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -2918,7 +2917,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="12" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -3102,7 +3101,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -3194,7 +3193,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="15" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -3306,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -3582,7 +3581,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -3630,7 +3629,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -3722,7 +3721,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -4090,7 +4089,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -4182,7 +4181,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -4274,7 +4273,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -4428,7 +4427,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -4493,7 +4492,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -4582,7 +4581,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -4858,7 +4857,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -4926,7 +4925,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -5018,7 +5017,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -5107,7 +5106,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -5288,7 +5287,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -5534,7 +5533,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -5705,7 +5704,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -5749,7 +5748,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -5924,7 +5923,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -5969,7 +5968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -6230,7 +6229,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="53" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -6313,7 +6312,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -6405,7 +6404,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -6494,7 +6493,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>339</v>
       </c>
@@ -6654,7 +6653,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -6796,7 +6795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>3</v>
       </c>
@@ -6879,7 +6878,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>299</v>
       </c>
@@ -6897,7 +6896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -7043,7 +7042,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -7123,7 +7122,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -7347,7 +7346,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -7404,7 +7403,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>338</v>
       </c>
@@ -7774,7 +7773,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>3</v>
       </c>
@@ -8047,7 +8046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -8200,7 +8199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>3</v>
       </c>
@@ -8313,7 +8312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -8611,7 +8610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>3</v>
       </c>
@@ -8776,7 +8775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>3</v>
       </c>
@@ -8865,7 +8864,7 @@
         <v>61.698541666666671</v>
       </c>
     </row>
-    <row r="100" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>3</v>
       </c>
@@ -8939,7 +8938,7 @@
         <v>44.217916666666667</v>
       </c>
     </row>
-    <row r="101" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>3</v>
       </c>
@@ -8972,7 +8971,7 @@
         <v>8.2202083333333356</v>
       </c>
     </row>
-    <row r="102" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>3</v>
       </c>
@@ -9005,7 +9004,7 @@
         <v>8.2526666666666664</v>
       </c>
     </row>
-    <row r="103" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>281</v>
       </c>
@@ -9109,7 +9108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>3</v>
       </c>
@@ -9145,7 +9144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -9254,7 +9253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>3</v>
       </c>
@@ -9571,7 +9570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>3</v>
       </c>
@@ -9654,7 +9653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>3</v>
       </c>
@@ -9819,7 +9818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>3</v>
       </c>
@@ -9871,7 +9870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>297</v>
       </c>
@@ -9886,7 +9885,7 @@
       </c>
       <c r="S129"/>
     </row>
-    <row r="130" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>3</v>
       </c>
@@ -9904,7 +9903,7 @@
       </c>
       <c r="S130"/>
     </row>
-    <row r="131" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>3</v>
       </c>
@@ -9925,7 +9924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>3</v>
       </c>
@@ -9943,7 +9942,7 @@
       </c>
       <c r="S132"/>
     </row>
-    <row r="133" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>3</v>
       </c>
@@ -10160,7 +10159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>3</v>
       </c>
@@ -10182,15 +10181,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AD141">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Long Fresh veg"/>
-        <filter val="Long Fruits"/>
-        <filter val="Soft Fruits"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:AD141"/>
   <mergeCells count="1">
     <mergeCell ref="F1:AC1"/>
   </mergeCells>

</xml_diff>